<commit_message>
Yasuo hoan thien chuc nang
</commit_message>
<xml_diff>
--- a/templateImportExcelMonHoc.xlsx
+++ b/templateImportExcelMonHoc.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23001"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\TotNghiep\CaoThangAngular\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DATN\CaoThangAngular\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86DA0981-9E9F-4F4E-98CB-D6385E85293C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{91656E51-A8C7-4601-BD34-1C69A65C61E6}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20736" windowHeight="11760"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,18 +36,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="13">
   <si>
     <t>tenMonHoc</t>
   </si>
   <si>
     <t>tenVietTat</t>
-  </si>
-  <si>
-    <t>tenTiengAnh</t>
-  </si>
-  <si>
-    <t>tenVietTatTiengAnh</t>
   </si>
   <si>
     <t>A</t>
@@ -87,7 +80,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -432,23 +425,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CAAF600-424D-477D-9D74-FF5F2C21230E}">
-  <dimension ref="A1:E5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.44140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -456,89 +449,59 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" t="s">
         <v>8</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" t="s">
-        <v>5</v>
-      </c>
-      <c r="E3" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" t="s">
-        <v>12</v>
-      </c>
-      <c r="D4" t="s">
-        <v>6</v>
-      </c>
-      <c r="E4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E5" t="s">
-        <v>7</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C8" xr:uid="{8C860A05-AE5E-4A2F-8375-6871CD89587B}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="C8">
       <formula1>maMonHoc</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C5" xr:uid="{443DEAC1-FF7A-45B8-A3C6-DD6CC1E8E27E}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C5">
       <formula1>maLoaiMonHoc</formula1>
     </dataValidation>
   </dataValidations>
@@ -547,51 +510,51 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E553222-CB76-4F60-9407-8ED8666F5C32}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
         <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H4 F8" xr:uid="{0CA67F56-725B-4CD6-A2F6-52898FBC59F0}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H2:H4 F8">
       <formula1>number</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1:A6" xr:uid="{04DA4E4E-DA5D-48BB-AF19-7091F52B2E13}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="A1:A6">
       <formula1>maLoaiMonHoc</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>